<commit_message>
feat(Avtls): 添加 2View 功能支持
- 新增 2View 功能的相关代码和菜单加载逻辑
- 实现了多视图切换和视图控制的功能
- 优化了视图显示和用户交互体验
</commit_message>
<xml_diff>
--- a/08ARK_XEE_纬地图层.xlsx
+++ b/08ARK_XEE_纬地图层.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tjueducn-my.sharepoint.com/personal/2013205268_tju_edu_cn/Documents/ProgramData/autocad/04 LISP程序/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{AF77934A-AF9A-465C-AD0E-CDD53CCC1EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEC6B9CD-48C8-46B8-9A75-948A89686824}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{AF77934A-AF9A-465C-AD0E-CDD53CCC1EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E435B57-0524-471C-AD15-E3D5C9BBBEE8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{EF619A6E-6F9F-458A-99A9-320127B085B0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF619A6E-6F9F-458A-99A9-320127B085B0}"/>
   </bookViews>
   <sheets>
     <sheet name="新建图层" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="55">
   <si>
     <t>线型</t>
   </si>
@@ -135,6 +135,75 @@
   </si>
   <si>
     <t>要素桩</t>
+  </si>
+  <si>
+    <t>Defpoints</t>
+  </si>
+  <si>
+    <t>SG-1道路-1临时道路</t>
+  </si>
+  <si>
+    <t>SG-1道路-1永久道路</t>
+  </si>
+  <si>
+    <t>SG-2支洞</t>
+  </si>
+  <si>
+    <t>SG-3场地</t>
+  </si>
+  <si>
+    <t>SG-3场地-供水</t>
+  </si>
+  <si>
+    <t>SG-3场地-系统</t>
+  </si>
+  <si>
+    <t>SG-4弃渣场</t>
+  </si>
+  <si>
+    <t>SG-4转存料场</t>
+  </si>
+  <si>
+    <t>SG-5料场</t>
+  </si>
+  <si>
+    <t>SG-8用地-1永久</t>
+  </si>
+  <si>
+    <t>SG-8用地-2临时</t>
+  </si>
+  <si>
+    <t>SG-8用地-弃渣场</t>
+  </si>
+  <si>
+    <t>SG-8用地-施工场地</t>
+  </si>
+  <si>
+    <t>SG-8用地-施工道路</t>
+  </si>
+  <si>
+    <t>SG-8用地-施工支洞</t>
+  </si>
+  <si>
+    <t>SG-civil</t>
+  </si>
+  <si>
+    <t>SG-测量范围</t>
+  </si>
+  <si>
+    <t>SG-水文断面</t>
+  </si>
+  <si>
+    <t>SG-图例</t>
+  </si>
+  <si>
+    <t>TK-图框</t>
+  </si>
+  <si>
+    <t>TK-图框-不打印</t>
+  </si>
+  <si>
+    <t>引出标注-Layer</t>
   </si>
 </sst>
 </file>
@@ -597,11 +666,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B6D133-15A1-4719-8933-A7DD412B1BE3}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G169"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
+      <pane ySplit="6" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -717,8 +786,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>18</v>
+      <c r="A10" s="4">
+        <v>0</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>19</v>
@@ -727,7 +796,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>3</v>
@@ -735,7 +804,7 @@
     </row>
     <row r="11" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>19</v>
@@ -744,7 +813,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>3</v>
@@ -752,16 +821,16 @@
     </row>
     <row r="12" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D12" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>3</v>
@@ -769,16 +838,16 @@
     </row>
     <row r="13" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D13" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>3</v>
@@ -786,16 +855,16 @@
     </row>
     <row r="14" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>3</v>
@@ -803,16 +872,16 @@
     </row>
     <row r="15" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D15" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>3</v>
@@ -820,16 +889,16 @@
     </row>
     <row r="16" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D16" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>3</v>
@@ -837,16 +906,16 @@
     </row>
     <row r="17" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D17" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>3</v>
@@ -854,7 +923,7 @@
     </row>
     <row r="18" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>19</v>
@@ -863,7 +932,7 @@
         <v>7</v>
       </c>
       <c r="D18" s="3">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>3</v>
@@ -871,7 +940,7 @@
     </row>
     <row r="19" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>19</v>
@@ -880,7 +949,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>3</v>
@@ -888,7 +957,7 @@
     </row>
     <row r="20" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>19</v>
@@ -897,7 +966,7 @@
         <v>7</v>
       </c>
       <c r="D20" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>3</v>
@@ -905,16 +974,16 @@
     </row>
     <row r="21" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="3">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D21" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>3</v>
@@ -922,29 +991,552 @@
     </row>
     <row r="22" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="3">
+        <v>7</v>
+      </c>
+      <c r="D22" s="3">
+        <v>3</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="3">
+        <v>7</v>
+      </c>
+      <c r="D23" s="3">
+        <v>3</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="3">
+        <v>7</v>
+      </c>
+      <c r="D24" s="3">
+        <v>3</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="3">
+        <v>7</v>
+      </c>
+      <c r="D25" s="3">
+        <v>3</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="3">
+        <v>7</v>
+      </c>
+      <c r="D26" s="3">
+        <v>3</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="3">
+        <v>7</v>
+      </c>
+      <c r="D27" s="3">
+        <v>3</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="3">
+        <v>7</v>
+      </c>
+      <c r="D28" s="3">
+        <v>3</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="3">
+        <v>7</v>
+      </c>
+      <c r="D29" s="3">
+        <v>3</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="3">
+        <v>7</v>
+      </c>
+      <c r="D30" s="3">
+        <v>3</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="3">
+        <v>7</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="3">
+        <v>7</v>
+      </c>
+      <c r="D32" s="3">
+        <v>3</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="3">
+        <v>7</v>
+      </c>
+      <c r="D33" s="3">
+        <v>3</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="3">
+        <v>8</v>
+      </c>
+      <c r="D34" s="3">
+        <v>3</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="3">
+        <v>7</v>
+      </c>
+      <c r="D35" s="3">
+        <v>3</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="3">
+        <v>7</v>
+      </c>
+      <c r="D36" s="3">
+        <v>3</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="3">
+        <v>7</v>
+      </c>
+      <c r="D37" s="3">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1</v>
+      </c>
+      <c r="D38" s="3">
+        <v>3</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="3">
+        <v>6</v>
+      </c>
+      <c r="D39" s="3">
+        <v>3</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="3">
+        <v>6</v>
+      </c>
+      <c r="D40" s="3">
+        <v>3</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="3">
+        <v>7</v>
+      </c>
+      <c r="D41" s="3">
+        <v>3</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="3">
+        <v>7</v>
+      </c>
+      <c r="D42" s="3">
+        <v>3</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="3">
+        <v>7</v>
+      </c>
+      <c r="D43" s="3">
+        <v>3</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="3">
+        <v>40</v>
+      </c>
+      <c r="D44" s="3">
+        <v>3</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="3">
+      <c r="B45" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="3">
         <v>6</v>
       </c>
-      <c r="D22" s="3">
-        <v>0</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D45" s="3">
+        <v>3</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="3">
+        <v>7</v>
+      </c>
+      <c r="D46" s="3">
+        <v>3</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection password="DEF0" sheet="1" objects="1" scenarios="1" formatRows="0" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <protectedRanges>

</xml_diff>